<commit_message>
adaptado al nuevo formulario de matriculacion
</commit_message>
<xml_diff>
--- a/prototipo/vistas/Archivos/Formulario_de_matriculacion.xlsx
+++ b/prototipo/vistas/Archivos/Formulario_de_matriculacion.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Griselda\Documents\MEGAsync\UNLa\Proyecto de Software\GestorDePedidos\prototipo\vistas\Archivos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="19420" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,16 +12,11 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nombre</t>
   </si>
@@ -46,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,19 +71,19 @@
   </fills>
   <borders count="2">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color indexed="64"/>
-      </end>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -118,7 +108,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -127,15 +117,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -177,7 +164,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,7 +199,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,22 +241,22 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="50%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35%">
-              <a:schemeClr val="phClr">
-                <a:tint val="37%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:tint val="15%"/>
-                <a:satMod val="350%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -277,22 +264,22 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:shade val="51%"/>
-                <a:satMod val="130%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80%">
-              <a:schemeClr val="phClr">
-                <a:shade val="93%"/>
-                <a:satMod val="130%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="94%"/>
-                <a:satMod val="135%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -303,8 +290,8 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95%"/>
-              <a:satMod val="105%"/>
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -327,7 +314,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38%"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -336,7 +323,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -345,7 +332,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -368,47 +355,47 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="40%"/>
-                <a:satMod val="350%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40%">
-              <a:schemeClr val="phClr">
-                <a:tint val="45%"/>
-                <a:shade val="99%"/>
-                <a:satMod val="350%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="20%"/>
-                <a:satMod val="255%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="-80%" r="50%" b="180%"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="80%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="30%"/>
-                <a:satMod val="200%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -420,23 +407,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="37.26953125" customWidth="1"/>
+    <col min="5" max="5" width="31.26953125" customWidth="1"/>
+    <col min="6" max="256" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,189 +441,189 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -649,24 +637,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="256" width="10.90625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="256" width="10.90625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>